<commit_message>
added list for Katie Beecroft
</commit_message>
<xml_diff>
--- a/1_Templated Entries/++A List RED ALERT .xlsx
+++ b/1_Templated Entries/++A List RED ALERT .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27560" yWindow="460" windowWidth="23640" windowHeight="27640" tabRatio="500"/>
+    <workbookView xWindow="2820" yWindow="460" windowWidth="23640" windowHeight="27640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3185,7 +3185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3421,7 +3421,6 @@
     <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3440,23 +3439,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3740,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="E350" sqref="E350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3784,7 +3767,7 @@
       <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="127" t="s">
+      <c r="E2" s="126" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="12">
@@ -3799,7 +3782,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="127" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="39" t="s">
@@ -4875,7 +4858,7 @@
       <c r="D56" s="99" t="s">
         <v>666</v>
       </c>
-      <c r="E56" s="123" t="s">
+      <c r="E56" s="118" t="s">
         <v>667</v>
       </c>
       <c r="F56" s="20">
@@ -5081,7 +5064,7 @@
       <c r="D66" s="63" t="s">
         <v>824</v>
       </c>
-      <c r="E66" s="124" t="s">
+      <c r="E66" s="123" t="s">
         <v>825</v>
       </c>
       <c r="F66" s="12">
@@ -5123,7 +5106,7 @@
       <c r="D68" s="32" t="s">
         <v>833</v>
       </c>
-      <c r="E68" s="125" t="s">
+      <c r="E68" s="124" t="s">
         <v>834</v>
       </c>
       <c r="F68" s="34">
@@ -5186,7 +5169,7 @@
       <c r="D71" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E71" s="127" t="s">
+      <c r="E71" s="126" t="s">
         <v>869</v>
       </c>
       <c r="F71" s="12">
@@ -5203,7 +5186,7 @@
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="15"/>
-      <c r="E72" s="129" t="s">
+      <c r="E72" s="128" t="s">
         <v>876</v>
       </c>
       <c r="F72" s="111">
@@ -5239,7 +5222,7 @@
       <c r="D74" s="15" t="s">
         <v>894</v>
       </c>
-      <c r="E74" s="124" t="s">
+      <c r="E74" s="123" t="s">
         <v>895</v>
       </c>
       <c r="F74" s="12">
@@ -5292,7 +5275,7 @@
       <c r="D77" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="126" t="s">
+      <c r="E77" s="125" t="s">
         <v>952</v>
       </c>
       <c r="F77" s="30">
@@ -13951,7 +13934,7 @@
     </row>
   </sheetData>
   <sortState ref="A1:G512">
-    <sortCondition sortBy="cellColor" ref="E1:E512" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="E1:E512" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Red Alert list
</commit_message>
<xml_diff>
--- a/1_Templated Entries/++A List RED ALERT .xlsx
+++ b/1_Templated Entries/++A List RED ALERT .xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenross/Desktop/REM/1_Templated Entries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LinkedModernisms/Desktop/REM/1_Templated Entries/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="460" windowWidth="23640" windowHeight="27640" tabRatio="500"/>
+    <workbookView xWindow="1840" yWindow="460" windowWidth="23640" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="956">
   <si>
     <t>Literature</t>
   </si>
@@ -2906,12 +2906,15 @@
   <si>
     <t>Bisso, Octavio Adolfo Montestruque, with Martin Fabbri Garcia, Katerine Ninoska Tapia, and Angeles Margarita Maqueira Yamasaki</t>
   </si>
+  <si>
+    <t>KT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3024,6 +3027,22 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3182,8 +3201,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3436,7 +3457,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -3721,10 +3744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G511"/>
+  <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
-      <selection activeCell="E350" sqref="E350"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3735,7 +3758,7 @@
     <col min="5" max="5" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3756,7 +3779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3777,7 +3800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>5</v>
       </c>
@@ -3798,7 +3821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
@@ -3818,8 +3841,11 @@
       <c r="G4" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
@@ -3837,8 +3863,11 @@
       <c r="G5" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
@@ -3859,7 +3888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
@@ -3878,7 +3907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>0</v>
       </c>
@@ -3899,7 +3928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -3918,7 +3947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>29</v>
       </c>
@@ -3938,8 +3967,11 @@
       <c r="G10" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
@@ -3960,7 +3992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
@@ -3979,7 +4011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>42</v>
       </c>
@@ -3999,8 +4031,11 @@
       <c r="G13" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>42</v>
       </c>
@@ -4020,8 +4055,11 @@
       <c r="G14" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>0</v>
       </c>
@@ -4041,8 +4079,11 @@
       <c r="G15" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
@@ -4061,7 +4102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>29</v>
       </c>
@@ -4082,7 +4123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -4103,7 +4144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>0</v>
       </c>
@@ -4123,8 +4164,11 @@
       <c r="G19" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -4144,8 +4188,11 @@
       <c r="G20" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
@@ -4163,8 +4210,11 @@
       <c r="G21" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>0</v>
       </c>
@@ -4184,8 +4234,11 @@
       <c r="G22" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>29</v>
       </c>
@@ -4206,7 +4259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>0</v>
       </c>
@@ -4227,7 +4280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>29</v>
       </c>
@@ -4248,7 +4301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>29</v>
       </c>
@@ -4269,7 +4322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9" t="s">
@@ -4287,8 +4340,11 @@
       <c r="G27" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>0</v>
       </c>
@@ -4308,8 +4364,11 @@
       <c r="G28" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -4330,7 +4389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -4349,7 +4408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
@@ -4368,7 +4427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>0</v>
       </c>
@@ -4389,7 +4448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9" t="s">
@@ -4407,8 +4466,11 @@
       <c r="G33" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9" t="s">
@@ -4424,8 +4486,11 @@
       <c r="G34" s="72" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>29</v>
       </c>
@@ -4445,8 +4510,11 @@
       <c r="G35" s="31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>0</v>
       </c>
@@ -4466,8 +4534,11 @@
       <c r="G36" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9" t="s">
@@ -4485,8 +4556,11 @@
       <c r="G37" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="14"/>
       <c r="C38" s="9" t="s">
@@ -4505,7 +4579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="9" t="s">
         <v>11</v>
@@ -4526,7 +4600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -4546,8 +4620,11 @@
       <c r="G40" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -4568,7 +4645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9" t="s">
@@ -4587,7 +4664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>29</v>
       </c>
@@ -4608,7 +4685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
@@ -4627,7 +4704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
@@ -4646,7 +4723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
       <c r="C46" s="9" t="s">
         <v>30</v>
@@ -4663,8 +4740,11 @@
       <c r="G46" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
@@ -4683,7 +4763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9" t="s">
@@ -13937,5 +14017,6 @@
     <sortCondition sortBy="cellColor" ref="E1:E512" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update red alert list and move three red entries to final
</commit_message>
<xml_diff>
--- a/1_Templated Entries/++A List RED ALERT .xlsx
+++ b/1_Templated Entries/++A List RED ALERT .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="17600" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="961">
   <si>
     <t>Literature</t>
   </si>
@@ -2910,9 +2910,6 @@
     <t>KT</t>
   </si>
   <si>
-    <t>RT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Done </t>
   </si>
   <si>
@@ -2923,13 +2920,16 @@
   </si>
   <si>
     <t>main repo</t>
+  </si>
+  <si>
+    <t>LM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3059,6 +3059,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="25">
@@ -3221,7 +3234,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3471,6 +3484,9 @@
     <xf numFmtId="0" fontId="13" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3761,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3836,7 +3852,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3860,7 +3876,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3882,7 +3898,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3906,7 +3922,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3928,7 +3944,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3952,7 +3968,7 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3974,7 +3990,7 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3998,7 +4014,7 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4022,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4044,7 +4060,7 @@
         <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4068,7 +4084,7 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4092,7 +4108,7 @@
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4116,7 +4132,7 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4138,7 +4154,7 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4162,7 +4178,7 @@
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4186,7 +4202,7 @@
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4210,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4234,7 +4250,7 @@
         <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4256,7 +4272,7 @@
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4280,7 +4296,7 @@
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4303,8 +4319,8 @@
       <c r="G23" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H23" t="s">
-        <v>960</v>
+      <c r="H23" s="129" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4327,8 +4343,8 @@
       <c r="G24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H24" t="s">
-        <v>960</v>
+      <c r="H24" s="129" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4352,7 +4368,7 @@
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4376,7 +4392,7 @@
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4398,7 +4414,7 @@
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4422,7 +4438,7 @@
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4446,7 +4462,7 @@
         <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4468,7 +4484,7 @@
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4490,7 +4506,7 @@
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4513,8 +4529,8 @@
       <c r="G32" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H32" t="s">
-        <v>960</v>
+      <c r="H32" s="129" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4536,7 +4552,7 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4555,8 +4571,8 @@
       <c r="G34" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="H34" t="s">
-        <v>959</v>
+      <c r="H34" s="131" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -4580,7 +4596,7 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4604,7 +4620,7 @@
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4626,7 +4642,7 @@
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4648,7 +4664,7 @@
         <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4672,7 +4688,7 @@
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4695,8 +4711,8 @@
       <c r="G40" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H40" t="s">
-        <v>960</v>
+      <c r="H40" s="129" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4720,7 +4736,7 @@
         <v>4</v>
       </c>
       <c r="H41" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4742,7 +4758,7 @@
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4766,7 +4782,7 @@
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4787,8 +4803,8 @@
       <c r="G44" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H44" t="s">
-        <v>959</v>
+      <c r="H44" s="131" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4810,7 +4826,7 @@
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4830,7 +4846,7 @@
       <c r="G46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="131" t="s">
         <v>955</v>
       </c>
     </row>
@@ -4852,8 +4868,8 @@
       <c r="G47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H47" t="s">
-        <v>960</v>
+      <c r="H47" s="129" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4875,7 +4891,7 @@
         <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4898,6 +4914,9 @@
       <c r="G49" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H49" s="130" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
@@ -4918,6 +4937,9 @@
       </c>
       <c r="G50" s="13" t="s">
         <v>4</v>
+      </c>
+      <c r="H50" s="130" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4940,6 +4962,9 @@
       <c r="G51" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H51" s="129" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
@@ -4962,7 +4987,7 @@
         <v>4</v>
       </c>
       <c r="H52" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4985,6 +5010,9 @@
       <c r="G53" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H53" s="130" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
@@ -5005,6 +5033,9 @@
       </c>
       <c r="G54" s="13" t="s">
         <v>4</v>
+      </c>
+      <c r="H54" s="130" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5026,7 +5057,7 @@
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5049,6 +5080,9 @@
       <c r="G56" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H56" s="131" t="s">
+        <v>958</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
@@ -5071,7 +5105,7 @@
         <v>4</v>
       </c>
       <c r="H57" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5095,7 +5129,7 @@
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5119,7 +5153,7 @@
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5142,6 +5176,9 @@
       <c r="G60" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H60" s="130" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
@@ -5164,7 +5201,7 @@
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5186,6 +5223,9 @@
       </c>
       <c r="G62" s="13" t="s">
         <v>4</v>
+      </c>
+      <c r="H62" s="131" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5207,7 +5247,7 @@
         <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5231,7 +5271,7 @@
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5253,6 +5293,9 @@
       </c>
       <c r="G65" s="13" t="s">
         <v>4</v>
+      </c>
+      <c r="H65" s="130" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5273,6 +5316,9 @@
       <c r="G66" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H66" s="130" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
@@ -5295,7 +5341,7 @@
         <v>4</v>
       </c>
       <c r="H67" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5318,6 +5364,9 @@
       <c r="G68" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H68" s="131" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -5340,7 +5389,7 @@
         <v>4</v>
       </c>
       <c r="H69" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5364,7 +5413,7 @@
         <v>4</v>
       </c>
       <c r="H70" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5480,7 +5529,9 @@
         <v>0</v>
       </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="3"/>
+      <c r="C77" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D77" s="114" t="s">
         <v>12</v>
       </c>
@@ -5492,6 +5543,9 @@
       </c>
       <c r="G77" s="31" t="s">
         <v>4</v>
+      </c>
+      <c r="H77" s="130" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5512,6 +5566,9 @@
       <c r="G78" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H78" s="130" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
@@ -5534,7 +5591,7 @@
         <v>4</v>
       </c>
       <c r="H79" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7182,7 +7239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="8"/>
       <c r="B161" s="9"/>
       <c r="C161" s="9" t="s">
@@ -7200,8 +7257,11 @@
       <c r="G161" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H161" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
         <v>0</v>
       </c>
@@ -7222,7 +7282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
         <v>65</v>
       </c>
@@ -7243,7 +7303,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="s">
         <v>0</v>
       </c>
@@ -7262,7 +7322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="8"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9" t="s">
@@ -7281,7 +7341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="8"/>
       <c r="B166" s="9"/>
       <c r="C166" s="9" t="s">
@@ -7300,7 +7360,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>0</v>
       </c>
@@ -7319,7 +7379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
         <v>299</v>
       </c>
@@ -7340,7 +7400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
         <v>0</v>
       </c>
@@ -7361,7 +7421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
         <v>0</v>
       </c>
@@ -7382,7 +7442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
         <v>0</v>
       </c>
@@ -7403,7 +7463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>0</v>
       </c>
@@ -7424,7 +7484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
         <v>42</v>
       </c>
@@ -7445,7 +7505,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="8"/>
       <c r="B174" s="9"/>
       <c r="C174" s="9" t="s">
@@ -7464,7 +7524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="8"/>
       <c r="B175" s="9"/>
       <c r="C175" s="9" t="s">
@@ -7483,7 +7543,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
update red list and finalize W
</commit_message>
<xml_diff>
--- a/1_Templated Entries/++A List RED ALERT .xlsx
+++ b/1_Templated Entries/++A List RED ALERT .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="640" windowWidth="17600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="3620" yWindow="540" windowWidth="14640" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2374" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="963">
   <si>
     <t>Literature</t>
   </si>
@@ -2921,12 +2921,21 @@
   <si>
     <t>LM</t>
   </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>kt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3077,6 +3086,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="25">
@@ -3239,7 +3263,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3493,6 +3517,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3783,8 +3810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3836,6 +3863,9 @@
       <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H2" s="129" t="s">
+        <v>958</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
@@ -4325,8 +4355,8 @@
       <c r="G23" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="129" t="s">
-        <v>958</v>
+      <c r="H23" s="133" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4536,7 +4566,7 @@
         <v>4</v>
       </c>
       <c r="H32" s="129" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4577,7 +4607,7 @@
       <c r="G34" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="H34" s="131" t="s">
+      <c r="H34" s="135" t="s">
         <v>957</v>
       </c>
     </row>
@@ -4717,8 +4747,8 @@
       <c r="G40" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="129" t="s">
-        <v>958</v>
+      <c r="H40" s="134" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4853,7 +4883,7 @@
         <v>4</v>
       </c>
       <c r="H46" s="132" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4874,8 +4904,8 @@
       <c r="G47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H47" s="129" t="s">
-        <v>958</v>
+      <c r="H47" s="134" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4920,8 +4950,8 @@
       <c r="G49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H49" s="130" t="s">
-        <v>958</v>
+      <c r="H49" s="134" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4968,8 +4998,8 @@
       <c r="G51" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H51" s="129" t="s">
-        <v>958</v>
+      <c r="H51" s="134" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5016,8 +5046,8 @@
       <c r="G53" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H53" s="130" t="s">
-        <v>958</v>
+      <c r="H53" s="134" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5040,8 +5070,8 @@
       <c r="G54" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H54" s="130" t="s">
-        <v>958</v>
+      <c r="H54" s="134" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5086,7 +5116,7 @@
       <c r="G56" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H56" s="131" t="s">
+      <c r="H56" s="135" t="s">
         <v>957</v>
       </c>
     </row>
@@ -5182,8 +5212,8 @@
       <c r="G60" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H60" s="130" t="s">
-        <v>958</v>
+      <c r="H60" s="134" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5230,7 +5260,7 @@
       <c r="G62" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H62" s="131" t="s">
+      <c r="H62" s="135" t="s">
         <v>957</v>
       </c>
     </row>
@@ -5371,7 +5401,7 @@
         <v>4</v>
       </c>
       <c r="H68" s="131" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5512,6 +5542,9 @@
       <c r="G75" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H75" t="s">
+        <v>961</v>
+      </c>
     </row>
     <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
@@ -5529,6 +5562,7 @@
       <c r="G76" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="H76" s="129"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
@@ -5572,8 +5606,8 @@
       <c r="G78" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H78" s="130" t="s">
-        <v>958</v>
+      <c r="H78" s="134" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">

</xml_diff>